<commit_message>
Research papers_LLms in e-commerce +Knowledge graph document
</commit_message>
<xml_diff>
--- a/Research/Research Documentation.xlsx
+++ b/Research/Research Documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anu_nambiar/Git/Msc_Project/Research/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67AD2F83-2BCC-6845-95E7-A5797D4A44BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B5161A5-C362-DD4E-80A2-E6BF0B950876}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="660" windowWidth="25440" windowHeight="15140" xr2:uid="{F43E4A0F-1D12-9D48-9EA7-9FF0C7403B2F}"/>
+    <workbookView xWindow="80" yWindow="660" windowWidth="25440" windowHeight="15120" xr2:uid="{F43E4A0F-1D12-9D48-9EA7-9FF0C7403B2F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,15 +35,430 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+  <si>
+    <t>Content summary/key finding</t>
+  </si>
+  <si>
+    <t>Paper Name</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/1706.03762</t>
+  </si>
+  <si>
+    <t>Sl.No</t>
+  </si>
+  <si>
+    <r>
+      <t>Vaswani, A., 2017. Attention is all you need. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Advances in Neural Information Processing Systems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Citation(Harvard)</t>
+  </si>
+  <si>
+    <t>Attention is all you need</t>
+  </si>
+  <si>
+    <r>
+      <t>Arslan, M., Munawar, S. and Cruz, C., 2024. Business insights using RAG–LLMs: a review and case study. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Journal of Decision Systems</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, pp.1-30.</t>
+    </r>
+  </si>
+  <si>
+    <t>Business insights using RAG–LLMs</t>
+  </si>
+  <si>
+    <t>https://www.tandfonline.com/doi/full/10.1080/12460125.2024.2410040</t>
+  </si>
+  <si>
+    <r>
+      <t>Cuconasu, F., Trappolini, G., Siciliano, F., Filice, S., Campagnano, C., Maarek, Y., Tonellotto, N. and Silvestri, F., 2024, July. The power of noise: Redefining retrieval for rag systems. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceedings of the 47th International ACM SIGIR Conference on Research and Development in Information Retrieval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (pp. 719-729).</t>
+    </r>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/3626772.3657834</t>
+  </si>
+  <si>
+    <r>
+      <t>Liu, J., Lin, J. and Liu, Y., 2024. How much can rag help the reasoning of llm?. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv preprint arXiv:2410.02338</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>How much can rag help the reasoning of llm?</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2410.02338</t>
+  </si>
+  <si>
+    <r>
+      <t>Mansurova, A., Mansurova, A. and Nugumanova, A., 2024. QA-RAG: Exploring LLM Reliance on External Knowledge. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Big Data and Cognitive Computing</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>(9), p.115.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.mdpi.com/2504-2289/8/9/115</t>
+  </si>
+  <si>
+    <t>Exploring LLM Reliance on External Knowledge</t>
+  </si>
+  <si>
+    <t>The power of noise: Redefining retrieval for rag systems</t>
+  </si>
+  <si>
+    <r>
+      <t>Wu, K., Wu, E. and Zou, J., 2024. How faithful are RAG models? Quantifying the tug-of-war between RAG and LLMs' internal prior. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv e-prints</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, pp.arXiv-2404.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://ui.adsabs.harvard.edu/abs/2024arXiv240410198W/abstract</t>
+  </si>
+  <si>
+    <t>How faithful are RAG models? Quantifying the tug-of-war between RAG and LLMs' internal prio</t>
+  </si>
+  <si>
+    <r>
+      <t>Yu, T., Xu, A. and Akkiraju, R., 2024. In defense of rag in the era of long-context language models. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv preprint arXiv:2409.01666</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2409.01666</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> In defense of rag in the era of long-context language models.</t>
+  </si>
+  <si>
+    <t>https://dl.acm.org/doi/abs/10.1145/3626772.3657935</t>
+  </si>
+  <si>
+    <r>
+      <t>Huly, O., Pogrebinsky, I., Carmel, D., Kurland, O. and Maarek, Y., 2024, July. Old IR Methods Meet RAG. In </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Proceedings of the 47th International ACM SIGIR Conference on Research and Development in Information Retrieval</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t> (pp. 2559-2563).</t>
+    </r>
+  </si>
+  <si>
+    <t>Old IR Methods Meet RAG.</t>
+  </si>
+  <si>
+    <t>https://arxiv.org/abs/2406.18064</t>
+  </si>
+  <si>
+    <r>
+      <t>Wang, Y., Hernandez, A.G., Kyslyi, R. and Kersting, N., 2024. Evaluating quality of answers for Retrieval-Augmented Generation: A strong LLM is all you need. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv preprint arXiv:2406.18064</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Evaluating quality of answers for Retrieval-Augmented Generation: A strong LLM is all you need</t>
+  </si>
+  <si>
+    <r>
+      <t>Arslan, M., Ghanem, H., Munawar, S. and Cruz, C., 2024. A Survey on RAG with LLMs. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Procedia Computer Science</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>246</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>, pp.3781-3790.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S1877050924021860</t>
+  </si>
+  <si>
+    <t>A Survey on RAG with LLMs</t>
+  </si>
+  <si>
+    <r>
+      <t>Zhou, Y., Liu, Y., Li, X., Jin, J., Qian, H., Liu, Z., Li, C., Dou, Z., Ho, T.Y. and Yu, P.S., 2024. Trustworthiness in retrieval-augmented generation systems: A survey. </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>arXiv preprint arXiv:2409.10102</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color rgb="FF222222"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>https://www.zhouyujia.cn/attaches/TrustworthyRAG.pdf</t>
+  </si>
+  <si>
+    <t>Trustworthiness in retrieval-augmented generation systems: A survey</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="13"/>
+      <color rgb="FF222222"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -66,13 +481,170 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="18"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -83,6 +655,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E13C4BCF-5F7B-4E4D-A358-C8FCDB974673}" name="Table1" displayName="Table1" ref="A1:E19" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+  <autoFilter ref="A1:E19" xr:uid="{E13C4BCF-5F7B-4E4D-A358-C8FCDB974673}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{723A11C3-7931-CF46-8A0B-ED92C3A50FC1}" name="Sl.No" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{2586553F-CC81-3A42-ABBD-A6DF57B5D537}" name="Paper Name" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{19DC7A2B-5C38-B64B-9BFF-65083EE986D0}" name="Content summary/key finding" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{30104AB1-4963-2A4B-B643-A9B69E8CFA47}" name="Citation(Harvard)" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{68FB17EA-477C-294E-98FF-AEB3AA7604A2}" name="Link" dataDxfId="0"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -402,12 +988,269 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9ECA1AD-21D3-6F4E-B713-672193B8CDD6}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="39.83203125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="95.83203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="36.33203125" style="9" customWidth="1"/>
+    <col min="5" max="5" width="50.1640625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="20" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="62" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4">
+        <v>1</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+      <c r="A3" s="4">
+        <v>2</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="5"/>
+      <c r="D3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="198" x14ac:dyDescent="0.2">
+      <c r="A4" s="4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="72" x14ac:dyDescent="0.2">
+      <c r="A5" s="4">
+        <v>4</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+      <c r="A6" s="4">
+        <v>5</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+      <c r="A7" s="4">
+        <v>6</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+      <c r="A8" s="4">
+        <v>7</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A9" s="4">
+        <v>8</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="109" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4">
+        <v>9</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="90" x14ac:dyDescent="0.2">
+      <c r="A11" s="4">
+        <v>10</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="126" x14ac:dyDescent="0.2">
+      <c r="A12" s="4">
+        <v>11</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A13" s="4">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A14" s="4">
+        <v>13</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A15" s="4">
+        <v>14</v>
+      </c>
+      <c r="B15" s="6"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A16" s="4">
+        <v>15</v>
+      </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A17" s="4">
+        <v>16</v>
+      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A18" s="4">
+        <v>17</v>
+      </c>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="24" x14ac:dyDescent="0.2">
+      <c r="A19" s="4">
+        <v>18</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>